<commit_message>
updated validation and finalized chap 1
Chapter 1 scope is good. Completed definition of terms
chapter 3 changed validation and adjusted spacing
</commit_message>
<xml_diff>
--- a/iLearnCentral/Validation.xlsx
+++ b/iLearnCentral/Validation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Expriments</t>
   </si>
@@ -63,12 +63,6 @@
     <t>Learning Center have no IT support</t>
   </si>
   <si>
-    <t>Interview</t>
-  </si>
-  <si>
-    <t>Survey</t>
-  </si>
-  <si>
     <t>A dynamic learning center management system supporting different types of learning centers, i.e. day care, music, language studies</t>
   </si>
   <si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>Adding a module for educators employed by a center to keep track of lessons, update schedules, and integrate records to the system.</t>
+  </si>
+  <si>
+    <t>60% of the respondents agree to use the system</t>
   </si>
 </sst>
 </file>
@@ -671,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,13 +714,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -731,13 +728,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -754,18 +751,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,13 +784,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>